<commit_message>
Report and Data updated
</commit_message>
<xml_diff>
--- a/ECE 478 - Project 1 Data.xlsx
+++ b/ECE 478 - Project 1 Data.xlsx
@@ -436,12 +436,26 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
+                  <a:sysClr val="window" lastClr="FFFFFF">
                     <a:lumMod val="95000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:effectLst>
                   <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
@@ -457,8 +471,35 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput of Node A</a:t>
+              <a:t>Average Throughput of Node A While </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1800">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -474,12 +515,26 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
+                <a:sysClr val="window" lastClr="FFFFFF">
                   <a:lumMod val="95000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:effectLst>
                 <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
@@ -1246,7 +1301,31 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Index Twice Rate</a:t>
+              <a:t> Index</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = 2λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2023,9 +2102,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput of Node C</a:t>
+              <a:t>Throughput of Node C </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2797,9 +2907,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput of Node A Twice Rate</a:t>
+              <a:t>Throughput of Node A </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = 2λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3634,9 +3775,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Throughput of Node C Twice Rate</a:t>
+              <a:t>Throughput of Node C </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = 2λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -4406,9 +4578,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Collisions of Node A</a:t>
+              <a:t>Collisions of Node A </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5177,9 +5380,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Collisions of Node C</a:t>
+              <a:t>Collisions of Node C </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -5947,9 +6181,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Collisions of Node A Twice Rate</a:t>
+              <a:t>Collisions of Node A </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = 2λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6715,9 +6980,40 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average </a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Collisions of Node B Twice Rate</a:t>
+              <a:t>Collisions of Node B </a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = 2λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -7489,6 +7785,30 @@
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
               <a:t> Index</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> While λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>A</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> = λ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="-25000">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>C</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -14293,8 +14613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA88" sqref="AA88"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>

</xml_diff>

<commit_message>
All graphs on word doc
</commit_message>
<xml_diff>
--- a/ECE 478 - Project 1 Data.xlsx
+++ b/ECE 478 - Project 1 Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="13380" yWindow="0" windowWidth="15420" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average Throughput of Node A: </a:t>
+              <a:t>Throughput of Node A: </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1800">
@@ -568,7 +568,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.105126209752866"/>
           <c:y val="0.127680878552972"/>
-          <c:w val="0.810887061613919"/>
+          <c:w val="0.659156446127022"/>
           <c:h val="0.73958635035151"/>
         </c:manualLayout>
       </c:layout>
@@ -769,6 +769,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -1174,6 +1175,71 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="6"/>
+              <c:spPr>
+                <a:gradFill rotWithShape="1">
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="103000"/>
+                        <a:lumMod val="102000"/>
+                        <a:tint val="94000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="50000">
+                      <a:schemeClr val="accent2">
+                        <a:satMod val="110000"/>
+                        <a:lumMod val="100000"/>
+                        <a:shade val="100000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="accent2">
+                        <a:lumMod val="99000"/>
+                        <a:satMod val="120000"/>
+                        <a:shade val="78000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+                <a:ln w="9525" cap="rnd">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst>
+                  <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                    <a:srgbClr val="000000">
+                      <a:alpha val="63000"/>
+                    </a:srgbClr>
+                  </a:outerShdw>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="lgDash"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:spPr>
               <a:noFill/>
@@ -1328,7 +1394,21 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2268,6 +2348,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -2477,7 +2558,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (frames/sec)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2590,16 +2671,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Average Fairness Index</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr cap="none"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>(# of Successful Pkts A / # of Successful Pkts C)</a:t>
+                  <a:t>Average Fairness Index (A/C)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2798,12 +2870,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Throughput of Node C:</a:t>
             </a:r>
@@ -3426,6 +3492,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -3583,9 +3650,8 @@
           <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3635,7 +3701,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3953,12 +4029,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Throughput of Node A:</a:t>
             </a:r>
@@ -4226,6 +4296,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -4641,6 +4712,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -4850,7 +4922,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5162,12 +5244,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Throughput of Node C:</a:t>
             </a:r>
@@ -5790,6 +5866,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -5999,7 +6076,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6317,12 +6404,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Collisions of Node A:</a:t>
             </a:r>
@@ -6941,6 +7022,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -7150,7 +7232,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7265,7 +7357,7 @@
                   <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Average  Number of Collisions</a:t>
+                  <a:t>Average  Number of Collisions (frames)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" cap="none" baseline="0"/>
               </a:p>
@@ -7465,12 +7557,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Collisions of Node C:</a:t>
             </a:r>
@@ -8089,6 +8175,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -8298,7 +8385,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8413,7 +8510,7 @@
                   <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>Average Number of Collisions</a:t>
+                  <a:t>Average Number of Collisions (frames)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8612,12 +8709,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Collisions of Node A:</a:t>
             </a:r>
@@ -9240,6 +9331,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -9449,7 +9541,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9562,7 +9664,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Average Number of COllisions</a:t>
+                  <a:t>Average Number of COllisions (frames)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9761,12 +9863,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Average </a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Collisions of Node C:</a:t>
             </a:r>
@@ -10385,6 +10481,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -10594,7 +10691,21 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10707,7 +10818,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Average Number of COllisions</a:t>
+                  <a:t>Average Number of COllisions (frames)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11528,6 +11639,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
+              <a:prstDash val="lgDash"/>
               <a:round/>
             </a:ln>
             <a:effectLst>
@@ -11737,7 +11849,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Transmission Rate (Mbps)</a:t>
+                  <a:t>Transmission Rate (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="1" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>frames/sec</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11850,16 +11972,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>Avverage Fairness Index</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr cap="none"/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" cap="none" baseline="0"/>
-                  <a:t>(# of Successful Pkts A / # of Successful Pkts C)</a:t>
+                  <a:t>Avverage Fairness Index (A/C)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -18086,8 +18199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AH30" sqref="AH30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edited data and graphs
</commit_message>
<xml_diff>
--- a/ECE 478 - Project 1 Data.xlsx
+++ b/ECE 478 - Project 1 Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13380" yWindow="0" windowWidth="15420" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="8980" yWindow="0" windowWidth="19820" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,10 +373,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,7 +389,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -397,10 +401,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1325,16 +1325,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.5988</c:v>
+                  <c:v>0.6012</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.1964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3796</c:v>
+                  <c:v>2.3928</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6316</c:v>
+                  <c:v>2.6796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1350,11 +1350,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1360599536"/>
-        <c:axId val="1325357552"/>
+        <c:axId val="1170794736"/>
+        <c:axId val="1071377488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1360599536"/>
+        <c:axId val="1170794736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,12 +1476,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1325357552"/>
+        <c:crossAx val="1071377488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1325357552"/>
+        <c:axId val="1071377488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1595,7 +1595,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1360599536"/>
+        <c:crossAx val="1170794736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2489,16 +2489,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.003488</c:v>
+                  <c:v>1.997002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.994013</c:v>
+                  <c:v>1.994554</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.740239</c:v>
+                  <c:v>2.905804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.763107</c:v>
+                  <c:v>3.687085</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2514,11 +2514,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430706144"/>
-        <c:axId val="1430710176"/>
+        <c:axId val="1198576336"/>
+        <c:axId val="1198580368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430706144"/>
+        <c:axId val="1198576336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2626,12 +2626,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430710176"/>
+        <c:crossAx val="1198580368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430710176"/>
+        <c:axId val="1198580368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2739,7 +2739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430706144"/>
+        <c:crossAx val="1198576336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3633,16 +3633,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.5988</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.194</c:v>
+                  <c:v>1.1976</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.388</c:v>
+                  <c:v>2.3868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6556</c:v>
+                  <c:v>2.6304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3657,11 +3657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1431313568"/>
-        <c:axId val="1431317600"/>
+        <c:axId val="1172458816"/>
+        <c:axId val="1172363680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1431313568"/>
+        <c:axId val="1172458816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,12 +3779,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1431317600"/>
+        <c:crossAx val="1172363680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1431317600"/>
+        <c:axId val="1172363680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3898,7 +3898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1431313568"/>
+        <c:crossAx val="1172458816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4856,13 +4856,13 @@
                   <c:v>1.1988</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3904</c:v>
+                  <c:v>2.3916</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8796</c:v>
+                  <c:v>3.9516</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2024</c:v>
+                  <c:v>4.1856</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4878,11 +4878,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430452656"/>
-        <c:axId val="1430455776"/>
+        <c:axId val="1173089120"/>
+        <c:axId val="1173093152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430452656"/>
+        <c:axId val="1173089120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5000,12 +5000,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430455776"/>
+        <c:crossAx val="1173093152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430455776"/>
+        <c:axId val="1173093152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5113,7 +5113,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430452656"/>
+        <c:crossAx val="1173089120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6007,16 +6007,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.5976</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.1988</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4148</c:v>
+                  <c:v>1.3596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.116</c:v>
+                  <c:v>1.1352</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6032,11 +6032,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430492032"/>
-        <c:axId val="1430496064"/>
+        <c:axId val="1173131600"/>
+        <c:axId val="1173135632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430492032"/>
+        <c:axId val="1173131600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6154,12 +6154,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430496064"/>
+        <c:crossAx val="1173135632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430496064"/>
+        <c:axId val="1173135632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6273,7 +6273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430492032"/>
+        <c:crossAx val="1173131600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7163,16 +7163,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>41.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>298.0</c:v>
+                  <c:v>229.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1447.0</c:v>
+                  <c:v>653.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>177.0</c:v>
+                  <c:v>154.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7188,11 +7188,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430529280"/>
-        <c:axId val="1430533312"/>
+        <c:axId val="1173180768"/>
+        <c:axId val="1173184800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430529280"/>
+        <c:axId val="1173180768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7310,12 +7310,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430533312"/>
+        <c:crossAx val="1173184800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430533312"/>
+        <c:axId val="1173184800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7426,7 +7426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430529280"/>
+        <c:crossAx val="1173180768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8316,16 +8316,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>41.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>298.0</c:v>
+                  <c:v>229.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1447.0</c:v>
+                  <c:v>653.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>177.0</c:v>
+                  <c:v>154.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8341,11 +8341,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430567744"/>
-        <c:axId val="1430571776"/>
+        <c:axId val="1173223344"/>
+        <c:axId val="1173227376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430567744"/>
+        <c:axId val="1173223344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8463,12 +8463,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430571776"/>
+        <c:crossAx val="1173227376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430571776"/>
+        <c:axId val="1173227376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8578,7 +8578,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430567744"/>
+        <c:crossAx val="1173223344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9472,16 +9472,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>115.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>882.0</c:v>
+                  <c:v>489.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159.0</c:v>
+                  <c:v>138.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>106.0</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9497,11 +9497,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430598400"/>
-        <c:axId val="1430602432"/>
+        <c:axId val="1173266272"/>
+        <c:axId val="1173270304"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430598400"/>
+        <c:axId val="1173266272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9619,12 +9619,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430602432"/>
+        <c:crossAx val="1173270304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430602432"/>
+        <c:axId val="1173270304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9732,7 +9732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430598400"/>
+        <c:crossAx val="1173266272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10622,16 +10622,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>115.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>882.0</c:v>
+                  <c:v>489.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>159.0</c:v>
+                  <c:v>138.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>106.0</c:v>
+                  <c:v>110.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10647,11 +10647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430633024"/>
-        <c:axId val="1430637056"/>
+        <c:axId val="1173306032"/>
+        <c:axId val="1173310064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430633024"/>
+        <c:axId val="1173306032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10773,12 +10773,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430637056"/>
+        <c:crossAx val="1173310064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430637056"/>
+        <c:axId val="1173310064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10886,7 +10886,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430633024"/>
+        <c:crossAx val="1173306032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11780,16 +11780,16 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.998769</c:v>
+                  <c:v>1.002402</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.002492</c:v>
+                  <c:v>0.998402</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.996541</c:v>
+                  <c:v>1.0023</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.991319</c:v>
+                  <c:v>1.018965</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11805,11 +11805,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1430671584"/>
-        <c:axId val="1430675616"/>
+        <c:axId val="1198534288"/>
+        <c:axId val="1198538320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1430671584"/>
+        <c:axId val="1198534288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11927,12 +11927,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430675616"/>
+        <c:crossAx val="1198538320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1430675616"/>
+        <c:axId val="1198538320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12040,7 +12040,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1430671584"/>
+        <c:crossAx val="1198534288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -17571,7 +17571,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17607,7 +17607,7 @@
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17645,7 +17645,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17683,7 +17683,7 @@
         <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17721,7 +17721,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000B000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17759,7 +17759,7 @@
         <xdr:cNvPr id="12" name="Chart 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17797,7 +17797,7 @@
         <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000D000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17835,7 +17835,7 @@
         <xdr:cNvPr id="14" name="Chart 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17873,7 +17873,7 @@
         <xdr:cNvPr id="15" name="Chart 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000F000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17911,7 +17911,7 @@
         <xdr:cNvPr id="16" name="Chart 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000010000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -18199,8 +18199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AH30" sqref="AH30"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18247,27 +18247,27 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="25"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="27"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="24" t="s">
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="27"/>
     </row>
     <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -18335,7 +18335,7 @@
         <v>0.59760000000000002</v>
       </c>
       <c r="J4" s="5">
-        <v>0.5988</v>
+        <v>0.60119999999999996</v>
       </c>
       <c r="K4" s="11">
         <v>50</v>
@@ -18344,7 +18344,7 @@
         <v>0.5988</v>
       </c>
       <c r="M4" s="12">
-        <v>0.5988</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -18383,7 +18383,7 @@
         <v>1.1879999999999999</v>
       </c>
       <c r="M5" s="12">
-        <v>1.194</v>
+        <v>1.1976</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -18413,7 +18413,7 @@
         <v>1.7796000000000001</v>
       </c>
       <c r="J6" s="5">
-        <v>2.3795999999999999</v>
+        <v>2.3927999999999998</v>
       </c>
       <c r="K6" s="11">
         <v>200</v>
@@ -18422,7 +18422,7 @@
         <v>1.8240000000000001</v>
       </c>
       <c r="M6" s="12">
-        <v>2.3879999999999999</v>
+        <v>2.3868</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -18452,7 +18452,7 @@
         <v>1.806</v>
       </c>
       <c r="J7" s="5">
-        <v>2.6316000000000002</v>
+        <v>2.6796000000000002</v>
       </c>
       <c r="K7" s="11">
         <v>300</v>
@@ -18461,7 +18461,7 @@
         <v>1.8804000000000001</v>
       </c>
       <c r="M7" s="12">
-        <v>2.6556000000000002</v>
+        <v>2.6303999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -18503,27 +18503,27 @@
       <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="24" t="s">
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="L10" s="26"/>
-      <c r="M10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="27"/>
     </row>
     <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -18574,7 +18574,7 @@
       <c r="C12" s="10">
         <v>1.1988000000000001</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="22">
         <v>50</v>
       </c>
       <c r="E12" s="10">
@@ -18600,7 +18600,7 @@
         <v>0.59640000000000004</v>
       </c>
       <c r="M12" s="12">
-        <v>0.59760000000000002</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -18630,7 +18630,7 @@
         <v>2.3028</v>
       </c>
       <c r="J13" s="10">
-        <v>2.3904000000000001</v>
+        <v>2.3915999999999999</v>
       </c>
       <c r="K13" s="11">
         <v>100</v>
@@ -18669,7 +18669,7 @@
         <v>2.5571999999999999</v>
       </c>
       <c r="J14" s="10">
-        <v>3.8795999999999999</v>
+        <v>3.9516</v>
       </c>
       <c r="K14" s="11">
         <v>200</v>
@@ -18678,7 +18678,7 @@
         <v>1.1208</v>
       </c>
       <c r="M14" s="12">
-        <v>1.4148000000000001</v>
+        <v>1.3595999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -18708,7 +18708,7 @@
         <v>2.2464</v>
       </c>
       <c r="J15" s="16">
-        <v>4.2023999999999999</v>
+        <v>4.1856</v>
       </c>
       <c r="K15" s="17">
         <v>300</v>
@@ -18717,7 +18717,7 @@
         <v>1.4339999999999999</v>
       </c>
       <c r="M15" s="18">
-        <v>1.1160000000000001</v>
+        <v>1.1352</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -18744,27 +18744,27 @@
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="24" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="25"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="27"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="24" t="s">
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="27"/>
     </row>
     <row r="19" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -18828,20 +18828,20 @@
       <c r="H20" s="9">
         <v>50</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="23">
         <v>654</v>
       </c>
-      <c r="J20" s="31">
-        <v>41</v>
+      <c r="J20" s="23">
+        <v>38</v>
       </c>
       <c r="K20" s="11">
         <v>50</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="23">
         <v>654</v>
       </c>
-      <c r="M20" s="31">
-        <v>41</v>
+      <c r="M20" s="23">
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -18867,20 +18867,20 @@
       <c r="H21" s="9">
         <v>100</v>
       </c>
-      <c r="I21" s="31">
+      <c r="I21" s="23">
         <v>1615</v>
       </c>
-      <c r="J21" s="31">
-        <v>298</v>
+      <c r="J21" s="23">
+        <v>229</v>
       </c>
       <c r="K21" s="11">
         <v>100</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="23">
         <v>1615</v>
       </c>
-      <c r="M21" s="31">
-        <v>298</v>
+      <c r="M21" s="23">
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -18906,59 +18906,59 @@
       <c r="H22" s="9">
         <v>200</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="23">
         <v>1549</v>
       </c>
-      <c r="J22" s="31">
-        <v>1447</v>
+      <c r="J22" s="23">
+        <v>653</v>
       </c>
       <c r="K22" s="11">
         <v>200</v>
       </c>
-      <c r="L22" s="31">
+      <c r="L22" s="23">
         <v>1549</v>
       </c>
-      <c r="M22" s="31">
-        <v>1447</v>
+      <c r="M22" s="23">
+        <v>653</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>300</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="23">
         <v>405</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="23">
         <v>421</v>
       </c>
       <c r="D23" s="11">
         <v>300</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="23">
         <v>405</v>
       </c>
-      <c r="F23" s="31">
+      <c r="F23" s="23">
         <v>421</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="9">
         <v>300</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="23">
         <v>1534</v>
       </c>
-      <c r="J23" s="31">
-        <v>177</v>
+      <c r="J23" s="23">
+        <v>154</v>
       </c>
       <c r="K23" s="11">
         <v>300</v>
       </c>
-      <c r="L23" s="31">
+      <c r="L23" s="23">
         <v>1534</v>
       </c>
-      <c r="M23" s="31">
-        <v>177</v>
+      <c r="M23" s="23">
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -19000,27 +19000,27 @@
       <c r="M25" s="14"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="24" t="s">
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="27"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="24" t="s">
+      <c r="I26" s="25"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="26"/>
-      <c r="M26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="27"/>
     </row>
     <row r="27" spans="1:13" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -19084,20 +19084,20 @@
       <c r="H28" s="9">
         <v>100</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="23">
         <v>1145</v>
       </c>
       <c r="J28" s="14">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="K28" s="11">
         <v>50</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="23">
         <v>1145</v>
       </c>
       <c r="M28" s="14">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -19123,20 +19123,20 @@
       <c r="H29" s="9">
         <v>200</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="23">
         <v>1584</v>
       </c>
       <c r="J29" s="14">
-        <v>882</v>
+        <v>489</v>
       </c>
       <c r="K29" s="11">
         <v>100</v>
       </c>
-      <c r="L29" s="31">
+      <c r="L29" s="23">
         <v>1584</v>
       </c>
       <c r="M29" s="14">
-        <v>882</v>
+        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -19162,20 +19162,20 @@
       <c r="H30" s="9">
         <v>400</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="23">
         <v>1537</v>
       </c>
       <c r="J30" s="14">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="K30" s="11">
         <v>200</v>
       </c>
-      <c r="L30" s="31">
+      <c r="L30" s="23">
         <v>1537</v>
       </c>
       <c r="M30" s="14">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -19205,7 +19205,7 @@
         <v>1538</v>
       </c>
       <c r="J31" s="20">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="K31" s="17">
         <v>300</v>
@@ -19214,24 +19214,24 @@
         <v>1538</v>
       </c>
       <c r="M31" s="20">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D33" s="27" t="s">
+      <c r="D33" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="3"/>
-      <c r="H33" s="27" t="s">
+      <c r="H33" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34" spans="4:10" ht="18" x14ac:dyDescent="0.25">
       <c r="D34" s="7" t="s">
@@ -19272,7 +19272,7 @@
         <v>0.99871699999999997</v>
       </c>
       <c r="J35" s="12">
-        <v>0.99876900000000002</v>
+        <v>1.002402</v>
       </c>
     </row>
     <row r="36" spans="4:10" x14ac:dyDescent="0.2">
@@ -19293,7 +19293,7 @@
         <v>1.00248</v>
       </c>
       <c r="J36" s="12">
-        <v>1.0024919999999999</v>
+        <v>0.99840200000000001</v>
       </c>
     </row>
     <row r="37" spans="4:10" x14ac:dyDescent="0.2">
@@ -19314,7 +19314,7 @@
         <v>0.97529900000000003</v>
       </c>
       <c r="J37" s="12">
-        <v>0.99654100000000001</v>
+        <v>1.0023</v>
       </c>
     </row>
     <row r="38" spans="4:10" x14ac:dyDescent="0.2">
@@ -19335,7 +19335,7 @@
         <v>0.96073500000000001</v>
       </c>
       <c r="J38" s="12">
-        <v>0.99131899999999995</v>
+        <v>1.0189649999999999</v>
       </c>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.2">
@@ -19348,17 +19348,17 @@
       <c r="J39" s="14"/>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="E40" s="23"/>
-      <c r="F40" s="25"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="27"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="23"/>
-      <c r="J40" s="25"/>
+      <c r="I40" s="28"/>
+      <c r="J40" s="27"/>
     </row>
     <row r="41" spans="4:10" ht="18" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
@@ -19399,7 +19399,7 @@
         <v>2.0051299999999999</v>
       </c>
       <c r="J42" s="12">
-        <v>2.0034879999999999</v>
+        <v>1.9970019999999999</v>
       </c>
     </row>
     <row r="43" spans="4:10" x14ac:dyDescent="0.2">
@@ -19420,7 +19420,7 @@
         <v>2.0650569999999999</v>
       </c>
       <c r="J43" s="12">
-        <v>1.994013</v>
+        <v>1.9945539999999999</v>
       </c>
     </row>
     <row r="44" spans="4:10" x14ac:dyDescent="0.2">
@@ -19441,7 +19441,7 @@
         <v>2.279903</v>
       </c>
       <c r="J44" s="12">
-        <v>2.7402389999999999</v>
+        <v>2.9058039999999998</v>
       </c>
     </row>
     <row r="45" spans="4:10" x14ac:dyDescent="0.2">
@@ -19462,11 +19462,17 @@
         <v>1.5656479999999999</v>
       </c>
       <c r="J45" s="18">
-        <v>3.7631070000000002</v>
+        <v>3.6870850000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="D40:F40"/>
@@ -19481,12 +19487,6 @@
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>